<commit_message>
minor improvements and bug fixes
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/tool.xlsx
+++ b/tests/testthat/fixtures/tool.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAP-338\Desktop\git\utilityR\tests\testthat\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reach\Desktop\Git\utilityR\tests\testthat\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C64340-0FBA-4090-B5DF-E6C323C31783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C11856-BEFD-4027-AFD7-74A45F81093A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="622" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="622" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="134">
   <si>
     <t>type</t>
   </si>
@@ -438,6 +438,9 @@
   </si>
   <si>
     <t>Dont select any other options if youve selected "Prefer not to answer" or "No impact on physical access to stores or marketplaces"</t>
+  </si>
+  <si>
+    <t>REACH</t>
   </si>
 </sst>
 </file>
@@ -557,7 +560,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -573,12 +576,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -598,9 +597,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -638,9 +637,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -673,26 +672,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -725,26 +707,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -920,18 +885,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="26.77734375" customWidth="1"/>
-    <col min="3" max="5" width="13.77734375" customWidth="1"/>
-    <col min="15" max="15" width="9.77734375" customWidth="1"/>
-    <col min="16" max="19" width="10.88671875" customWidth="1"/>
+    <col min="2" max="2" width="26.81640625" customWidth="1"/>
+    <col min="3" max="5" width="13.81640625" customWidth="1"/>
+    <col min="15" max="15" width="9.81640625" customWidth="1"/>
+    <col min="16" max="19" width="10.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -1157,105 +1122,96 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:20" s="11" customFormat="1">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:20">
+      <c r="A15" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="G15" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="H15" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="I15" s="12" t="s">
+      <c r="I15" t="s">
         <v>32</v>
       </c>
-      <c r="J15" s="12" t="s">
+      <c r="J15" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="12" t="s">
+      <c r="K15" t="s">
         <v>34</v>
       </c>
-      <c r="L15" s="12" t="s">
+      <c r="L15" t="s">
         <v>35</v>
       </c>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12" t="s">
+      <c r="P15" t="s">
         <v>108</v>
       </c>
-      <c r="Q15" s="12" t="s">
+      <c r="Q15" t="s">
         <v>132</v>
       </c>
-      <c r="R15" s="12" t="s">
+      <c r="R15" t="s">
         <v>109</v>
       </c>
-      <c r="S15" s="12" t="s">
+      <c r="S15" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="12" t="s">
+      <c r="A16" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" t="s">
         <v>111</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" t="s">
         <v>112</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" t="s">
         <v>113</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" t="s">
         <v>114</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" t="s">
         <v>115</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" t="s">
         <v>116</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" t="s">
         <v>32</v>
       </c>
-      <c r="J16" s="12" t="s">
+      <c r="J16" t="s">
         <v>33</v>
       </c>
-      <c r="K16" s="12" t="s">
+      <c r="K16" t="s">
         <v>34</v>
       </c>
-      <c r="L16" s="12" t="s">
+      <c r="L16" t="s">
         <v>35</v>
       </c>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12" t="s">
+      <c r="O16" t="s">
         <v>118</v>
       </c>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="12"/>
-      <c r="S16" s="12"/>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="7" t="s">
@@ -1274,18 +1230,18 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F4974"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C31" sqref="C31:C33"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="32.21875" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
-    <col min="3" max="5" width="17.88671875" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="32.1796875" customWidth="1"/>
+    <col min="2" max="2" width="33.6328125" customWidth="1"/>
+    <col min="3" max="5" width="17.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.36328125" customWidth="1"/>
+    <col min="7" max="7" width="9.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1540,10 +1496,10 @@
         <v>69</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>69</v>
+        <v>133</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>69</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1802,111 +1758,65 @@
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="16" t="s">
+      <c r="A31" t="s">
         <v>119</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" t="s">
         <v>120</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" t="s">
         <v>121</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" t="s">
         <v>122</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="E31" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="16" t="s">
+      <c r="A32" t="s">
         <v>119</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" t="s">
         <v>124</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" t="s">
         <v>125</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D32" t="s">
         <v>126</v>
       </c>
-      <c r="E32" s="16" t="s">
+      <c r="E32" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="16" t="s">
+      <c r="A33" t="s">
         <v>119</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B33" t="s">
         <v>128</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C33" t="s">
         <v>129</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D33" t="s">
         <v>130</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E33" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="16"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="16"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="16"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="16"/>
-      <c r="B37" s="16"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-    </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="16"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="16"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="16"/>
-      <c r="B40" s="16"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="16"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
     </row>
     <row r="109" ht="14.25" customHeight="1"/>
     <row r="113" ht="16.5" customHeight="1"/>
@@ -2048,10 +1958,10 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="2" width="34.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="1" max="2" width="34.36328125" customWidth="1"/>
+    <col min="3" max="3" width="17.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2094,14 +2004,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c228d1bd-650e-48eb-9f39-f684bd7bd257">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="fa0b5fe5-391f-41b6-811a-90e0518c7af2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2328,21 +2236,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c228d1bd-650e-48eb-9f39-f684bd7bd257">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="fa0b5fe5-391f-41b6-811a-90e0518c7af2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14732A80-0AB2-4E03-B790-B05DA57B3EBD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC9C6962-CA2C-4250-BDA6-104538449B01}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c228d1bd-650e-48eb-9f39-f684bd7bd257"/>
-    <ds:schemaRef ds:uri="fa0b5fe5-391f-41b6-811a-90e0518c7af2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2367,9 +2274,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC9C6962-CA2C-4250-BDA6-104538449B01}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14732A80-0AB2-4E03-B790-B05DA57B3EBD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c228d1bd-650e-48eb-9f39-f684bd7bd257"/>
+    <ds:schemaRef ds:uri="fa0b5fe5-391f-41b6-811a-90e0518c7af2"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>